<commit_message>
The database was updated and 77 businesses were re-arranged.
</commit_message>
<xml_diff>
--- a/materials/Бизнесы.xlsx
+++ b/materials/Бизнесы.xlsx
@@ -4,10 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Магазин 247" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист7" sheetId="8" r:id="rId2"/>
+    <sheet name="Заправка" sheetId="2" r:id="rId3"/>
+    <sheet name="Автосалоны" sheetId="3" r:id="rId4"/>
+    <sheet name="Оружейная" sheetId="4" r:id="rId5"/>
+    <sheet name="Одежда" sheetId="5" r:id="rId6"/>
+    <sheet name="Тату" sheetId="6" r:id="rId7"/>
+    <sheet name="Парики" sheetId="7" r:id="rId8"/>
+    <sheet name="Маски" sheetId="9" r:id="rId9"/>
+    <sheet name="Тюнинг" sheetId="10" r:id="rId10"/>
+    <sheet name="Автомойка" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
   <si>
     <t>№</t>
   </si>
@@ -37,13 +47,244 @@
   </si>
   <si>
     <t>Коржинаты выгрузки</t>
+  </si>
+  <si>
+    <t>1135.713 -982.809265 45.2958</t>
+  </si>
+  <si>
+    <t>-3041.0686 585.210754 6.78893042</t>
+  </si>
+  <si>
+    <t>-3243.70679 1001.39764 11.7107058</t>
+  </si>
+  <si>
+    <t>1729.65747 6416.007 33.9172249</t>
+  </si>
+  <si>
+    <t>1393.53516 3605.289 33.8609352</t>
+  </si>
+  <si>
+    <t>548.0653 2669.258 41.0365372</t>
+  </si>
+  <si>
+    <t>1165.71143 2709.35669 37.03772</t>
+  </si>
+  <si>
+    <t>374.325745 327.7953 102.446381</t>
+  </si>
+  <si>
+    <t>2555.58032 382.1431 107.50293</t>
+  </si>
+  <si>
+    <t>-1820.67212 792.438538 136.996246</t>
+  </si>
+  <si>
+    <t>-1222.58972 -906.994934 11.2063446</t>
+  </si>
+  <si>
+    <t>-47.2061539 -1756.49036 28.300993</t>
+  </si>
+  <si>
+    <t>Бот</t>
+  </si>
+  <si>
+    <t>823.117432 -1028.66064 25.1379471</t>
+  </si>
+  <si>
+    <t>616.311035 268.0051 101.969475</t>
+  </si>
+  <si>
+    <t>1182.55762 -334.524 68.05636</t>
+  </si>
+  <si>
+    <t>2006.10217 3770.21143 31.0607738</t>
+  </si>
+  <si>
+    <t>1208.30286 2662.54663 36.6899261</t>
+  </si>
+  <si>
+    <t>2577.606 362.69455 107.337257</t>
+  </si>
+  <si>
+    <t>176.371933 6601.90137 30.72888</t>
+  </si>
+  <si>
+    <t>1701.55518 6413.75049 31.629961</t>
+  </si>
+  <si>
+    <t>-2555.167 2330.76172 31.9400082</t>
+  </si>
+  <si>
+    <t>-2101.523 -319.928558 11.9077339</t>
+  </si>
+  <si>
+    <t>-32.6235275 -1111.76758 25.302351</t>
+  </si>
+  <si>
+    <t>-41.0745354 -1674.96631 28.330164</t>
+  </si>
+  <si>
+    <t>-803.292236 -224.015228 36.1051941</t>
+  </si>
+  <si>
+    <t>-177.0876 -1158.61987 22.6926613</t>
+  </si>
+  <si>
+    <t>-639.9547 297.048 81.33621</t>
+  </si>
+  <si>
+    <t>809.993835 -2157.224 28.4990139</t>
+  </si>
+  <si>
+    <t>-1308.6637 -395.171173 35.5757828</t>
+  </si>
+  <si>
+    <t>22.38435 -1107.29309 28.6770267</t>
+  </si>
+  <si>
+    <t>249.423172 -50.64652 68.82107</t>
+  </si>
+  <si>
+    <t>-661.971558 -935.3557 20.7092266</t>
+  </si>
+  <si>
+    <t>842.0606 -1033.65552 27.0748463</t>
+  </si>
+  <si>
+    <t>2567.62329 294.342468 107.614868</t>
+  </si>
+  <si>
+    <t>1693.68555 3759.96973 33.5853233</t>
+  </si>
+  <si>
+    <t>-330.255585 6084.13965 30.3347664</t>
+  </si>
+  <si>
+    <t>-1117.55811 2698.71729 17.4341469</t>
+  </si>
+  <si>
+    <t>4.56338358 6512.63525 30.7578487</t>
+  </si>
+  <si>
+    <t>425.338867 -806.0561 28.3711414</t>
+  </si>
+  <si>
+    <t>1693.51843 4822.854 40.94312</t>
+  </si>
+  <si>
+    <t>75.7154846 -1392.80188 28.2561436</t>
+  </si>
+  <si>
+    <t>1196.6748 2709.85352 37.1026039</t>
+  </si>
+  <si>
+    <t>125.845146 -223.120667 53.4378281</t>
+  </si>
+  <si>
+    <t>-709.913452 -153.204453 36.2951431</t>
+  </si>
+  <si>
+    <t>-822.232 -1073.6687 10.2080984</t>
+  </si>
+  <si>
+    <t>-1450.666 -237.52861 48.6902122</t>
+  </si>
+  <si>
+    <t>-3171.01929 1043.78076 19.7432117</t>
+  </si>
+  <si>
+    <t>-1101.14917 2710.15747 17.9878654</t>
+  </si>
+  <si>
+    <t>-163.061417 -302.664581 38.6132774</t>
+  </si>
+  <si>
+    <t>1322.8103 -1652.888 51.1553421</t>
+  </si>
+  <si>
+    <t>-1154.23267 -1426.39465 3.83446074</t>
+  </si>
+  <si>
+    <t>-3170.14185 1076.02893 19.7091846</t>
+  </si>
+  <si>
+    <t>-293.856 6200.67041 30.367115</t>
+  </si>
+  <si>
+    <t>1864.01489 3746.93872 31.9118824</t>
+  </si>
+  <si>
+    <t>323.0979 180.856659 102.466568</t>
+  </si>
+  <si>
+    <t>-280.03125 6227.557 30.5855274</t>
+  </si>
+  <si>
+    <t>1933.5365 3730.60181 31.73445</t>
+  </si>
+  <si>
+    <t>-815.404846 -182.401917 36.44893</t>
+  </si>
+  <si>
+    <t>-34.49098 -151.054169 55.96652</t>
+  </si>
+  <si>
+    <t>137.92012 -1709.88672 28.1816158</t>
+  </si>
+  <si>
+    <t>1211.08435 -474.581177 65.09804</t>
+  </si>
+  <si>
+    <t>-707.8512 -914.6364 18.0955887</t>
+  </si>
+  <si>
+    <t>-1337.23047 -1277.6958 3.75608921</t>
+  </si>
+  <si>
+    <t>-133.290359 -69.55716 54.2846642</t>
+  </si>
+  <si>
+    <t>-2963.144 454.539642 14.1952343</t>
+  </si>
+  <si>
+    <t>110.073448 6627.64355 30.66723</t>
+  </si>
+  <si>
+    <t>731.6122 -1088.7478 21.04901</t>
+  </si>
+  <si>
+    <t>-212.064713 -1323.9646 29.7703876</t>
+  </si>
+  <si>
+    <t>-338.426758 -136.95813 37.88963</t>
+  </si>
+  <si>
+    <t>-1154.64917 -2006.57727 12.0602551</t>
+  </si>
+  <si>
+    <t>-1795.883 805.5682 137.393341</t>
+  </si>
+  <si>
+    <t>-728.687744 -935.2535 17.8970051</t>
+  </si>
+  <si>
+    <t>-1335.74292 -2676.10059 12.824935</t>
+  </si>
+  <si>
+    <t>-699.6722 -935.1115 17.8939018</t>
+  </si>
+  <si>
+    <t>30.272789 -1391.75269 28.24023</t>
+  </si>
+  <si>
+    <t>170.848022 -1717.97864 28.17203</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +296,15 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -87,9 +337,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -370,48 +635,953 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
     <col min="4" max="4" width="29.140625" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>1000000</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="46.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="47" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="4" max="4" width="39.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="41" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="40.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>